<commit_message>
updated app requirements docs. refactored code to properly handle the add task functionality. other class structure improvements.
</commit_message>
<xml_diff>
--- a/Docs/Lab01/Lab01_ReviewReport.xlsx
+++ b/Docs/Lab01/Lab01_ReviewReport.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11027"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="11207"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudormihaita/IdeaProjects/vvss-tasks/Docs/lab01/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tudormihaita/IdeaProjects/vvss-tasks/Docs/Lab01/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A533FA1B-90DC-AD4A-A946-2CDBEDDF098F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FFE7854-62AB-914D-A537-201DE7601160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="17340" yWindow="940" windowWidth="17060" windowHeight="19840" tabRatio="650" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="26880" tabRatio="650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements Phase Defects" sheetId="7" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="95">
   <si>
     <t>do not print this form</t>
   </si>
@@ -105,34 +105,6 @@
   </si>
   <si>
     <t>Comments/ improvements</t>
-  </si>
-  <si>
-    <t>R01</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">Requirements are incomplete.  </t>
-    </r>
-    <r>
-      <rPr>
-        <i/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">                               It is not clearly specified how overlapping tasks are handled (for example, what happens if two tasks have intersecting time intervals).</t>
-    </r>
   </si>
   <si>
     <t>R04</t>
@@ -416,6 +388,53 @@
   </si>
   <si>
     <t>Effort to perform tool-based code analysis (hours): 0.8</t>
+  </si>
+  <si>
+    <t>R02</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Requirements are missing</t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">                                                            It is not clearly specified how the application handles error cases, such as when a user inputs invalid dates as start or end time for a task. The application could show an error to the user.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The user needs are inaduequately stated                                    </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>There's no mention of user goals. There should be a section stating the purpose of the application from the user's perspective. E.g.: Organizing their time by managing and tracking scheduled activities.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">                R06</t>
   </si>
 </sst>
 </file>
@@ -610,7 +629,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -691,6 +710,12 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1001,8 +1026,8 @@
   </sheetPr>
   <dimension ref="A1:J27"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1165,17 +1190,17 @@
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
     </row>
-    <row r="10" spans="1:10" ht="64" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A10" s="16"/>
       <c r="B10" s="17">
         <v>1</v>
       </c>
       <c r="C10" s="21" t="s">
-        <v>22</v>
+        <v>91</v>
       </c>
       <c r="D10" s="1"/>
       <c r="E10" s="20" t="s">
-        <v>23</v>
+        <v>92</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -1190,11 +1215,11 @@
         <v>2</v>
       </c>
       <c r="C11" s="22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D11" s="1"/>
       <c r="E11" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -1209,11 +1234,11 @@
         <v>3</v>
       </c>
       <c r="C12" s="22" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D12" s="1"/>
       <c r="E12" s="20" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -1221,15 +1246,19 @@
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:10" ht="80" x14ac:dyDescent="0.2">
       <c r="A13" s="16"/>
       <c r="B13" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C13" s="1"/>
+      <c r="C13" s="38" t="s">
+        <v>94</v>
+      </c>
       <c r="D13" s="1"/>
-      <c r="E13" s="2"/>
+      <c r="E13" s="37" t="s">
+        <v>93</v>
+      </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
@@ -1365,7 +1394,7 @@
     <row r="27" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B27" s="16"/>
       <c r="C27" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D27" s="11"/>
       <c r="E27" s="1">
@@ -1393,7 +1422,7 @@
   </sheetPr>
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
@@ -1428,7 +1457,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="25" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -1468,7 +1497,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="29" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E4" s="29"/>
       <c r="F4" s="16"/>
@@ -1487,10 +1516,10 @@
       <c r="A5" s="16"/>
       <c r="B5" s="16"/>
       <c r="C5" s="6" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="D5" s="30" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="E5" s="31"/>
       <c r="F5" s="16"/>
@@ -1512,7 +1541,7 @@
         <v>15</v>
       </c>
       <c r="D6" s="23" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="E6" s="23"/>
       <c r="F6" s="16"/>
@@ -1563,13 +1592,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>36</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -1584,13 +1613,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -1605,13 +1634,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -1626,13 +1655,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -1647,13 +1676,13 @@
         <v>5</v>
       </c>
       <c r="C14" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>44</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>45</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="F14" s="16"/>
       <c r="G14" s="16"/>
@@ -1784,7 +1813,7 @@
     <row r="28" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B28" s="16"/>
       <c r="C28" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D28" s="11"/>
       <c r="E28" s="1">
@@ -1847,7 +1876,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="25" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -1887,7 +1916,7 @@
         <v>7</v>
       </c>
       <c r="D4" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E4" s="32"/>
       <c r="F4" s="16"/>
@@ -1909,7 +1938,7 @@
         <v>11</v>
       </c>
       <c r="D5" s="33" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E5" s="34"/>
       <c r="F5" s="16"/>
@@ -1982,13 +2011,13 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="D10" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="F10" s="16"/>
       <c r="G10" s="16"/>
@@ -2003,13 +2032,13 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>53</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="F11" s="16"/>
       <c r="G11" s="16"/>
@@ -2024,13 +2053,13 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>56</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>58</v>
       </c>
       <c r="F12" s="16"/>
       <c r="G12" s="16"/>
@@ -2045,13 +2074,13 @@
         <v>4</v>
       </c>
       <c r="C13" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F13" s="16"/>
       <c r="G13" s="16"/>
@@ -2233,7 +2262,7 @@
     <row r="32" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B32" s="16"/>
       <c r="C32" s="10" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D32" s="11"/>
       <c r="E32" s="1">
@@ -2297,7 +2326,7 @@
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="16"/>
       <c r="B2" s="25" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C2" s="25"/>
       <c r="D2" s="25"/>
@@ -2334,7 +2363,7 @@
       <c r="A4" s="16"/>
       <c r="B4" s="16"/>
       <c r="C4" s="14" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D4" s="32"/>
       <c r="E4" s="32"/>
@@ -2357,7 +2386,7 @@
         <v>15</v>
       </c>
       <c r="D5" s="23" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5" s="23"/>
       <c r="F5" s="16"/>
@@ -2394,16 +2423,16 @@
         <v>18</v>
       </c>
       <c r="C9" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="E9" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="F9" s="9" t="s">
         <v>65</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>66</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>67</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="16"/>
@@ -2416,16 +2445,16 @@
         <v>1</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E10" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>69</v>
-      </c>
-      <c r="E10" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>71</v>
       </c>
       <c r="G10" s="16"/>
       <c r="H10" s="16"/>
@@ -2439,16 +2468,16 @@
         <v>2</v>
       </c>
       <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="F11" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="E11" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="F11" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="G11" s="16"/>
       <c r="H11" s="16"/>
@@ -2462,16 +2491,16 @@
         <v>3</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E12" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="F12" s="2" t="s">
         <v>77</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>79</v>
       </c>
       <c r="G12" s="16"/>
       <c r="H12" s="16"/>
@@ -2485,16 +2514,16 @@
         <v>4</v>
       </c>
       <c r="C13" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="E13" s="2" t="s">
         <v>80</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>81</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>83</v>
       </c>
       <c r="G13" s="16"/>
       <c r="H13" s="16"/>
@@ -2508,16 +2537,16 @@
         <v>5</v>
       </c>
       <c r="C14" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E14" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D14" s="2" t="s">
+      <c r="F14" s="2" t="s">
         <v>85</v>
-      </c>
-      <c r="E14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="F14" s="2" t="s">
-        <v>87</v>
       </c>
       <c r="G14" s="16"/>
       <c r="H14" s="16"/>
@@ -2531,16 +2560,16 @@
         <v>6</v>
       </c>
       <c r="C15" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="F15" s="2" t="s">
         <v>89</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>91</v>
       </c>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
@@ -2705,7 +2734,7 @@
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B32" s="16"/>
       <c r="C32" s="35" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="D32" s="36"/>
       <c r="E32" s="36"/>

</xml_diff>